<commit_message>
Adicionadas as informações anteriormente coletadas
</commit_message>
<xml_diff>
--- a/Dot Project EAP/4. System Management/Entrega Final/Escopo-Qualidade.xlsx
+++ b/Dot Project EAP/4. System Management/Entrega Final/Escopo-Qualidade.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories Planejadas" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,120 @@
     <sheet name="APF - Detalhada" sheetId="5" r:id="rId5"/>
     <sheet name="Grafico - APF" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Stories</t>
+  </si>
+  <si>
+    <t>Prioridade</t>
+  </si>
+  <si>
+    <t>User Story Point</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Observações</t>
+  </si>
+  <si>
+    <t>Conclusão</t>
+  </si>
+  <si>
+    <t>Funçao Tipo de Dado</t>
+  </si>
+  <si>
+    <t>Tipo de Função</t>
+  </si>
+  <si>
+    <t>Pontos de Função</t>
+  </si>
+  <si>
+    <t>EAP</t>
+  </si>
+  <si>
+    <t>Equipe</t>
+  </si>
+  <si>
+    <t>Projeto</t>
+  </si>
+  <si>
+    <t>Entregas</t>
+  </si>
+  <si>
+    <t>Atividades</t>
+  </si>
+  <si>
+    <t>Membro</t>
+  </si>
+  <si>
+    <t>Indicativo do Tamanho</t>
+  </si>
+  <si>
+    <t>ALI</t>
+  </si>
+  <si>
+    <t>Produtividade 10 hr/PF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10hr X PF`s </t>
+  </si>
+  <si>
+    <t>hrs</t>
+  </si>
+  <si>
+    <t>Criar o primeiro nó 0 cujo campo será preechido pelo nome do projeto</t>
+  </si>
+  <si>
+    <t>Criar os filhos do nó 0 que serão os pacotes de trabalho</t>
+  </si>
+  <si>
+    <t>Visualizar todos os campos da EAP criada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excluir qualquer nó, com exceção de nó 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alterar o conteúdo do campo </t>
+  </si>
+  <si>
+    <t>Cada nó deve criar novos filhos, formando uma hierarquia</t>
+  </si>
+  <si>
+    <t>Persistir dados da EAP criada/ alterada</t>
+  </si>
+  <si>
+    <t>Criar ultimo nível que será de esforço</t>
+  </si>
+  <si>
+    <t>Regras de Negócio</t>
+  </si>
+  <si>
+    <t>RN1</t>
+  </si>
+  <si>
+    <t>A EAP deve possuir no maximo 5 níveis, sendo o nível 0 o nome do projeto e o ultimo nível e de esforço</t>
+  </si>
+  <si>
+    <t>RN2</t>
+  </si>
+  <si>
+    <t>Ao excluir um nó, os nós de hierarquia maior ou igual ao nó a ser excluido, também devem ser excluidos</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +135,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -45,12 +175,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,24 +586,399 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="67.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="67.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="92.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="J1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>40</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>40</v>
+      </c>
+      <c r="E4" s="7">
+        <v>2</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="7">
+        <v>3</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="7">
+        <v>3</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="7">
+        <v>4</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="7">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -388,12 +997,124 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
+        <f>SUM(C2:C7)</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <f>C10*10</f>
+        <v>2100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -414,7 +1135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>